<commit_message>
update commit for hcm2
</commit_message>
<xml_diff>
--- a/HCM2/input/9036_03043900_2022_Student Datasheet.xlsx
+++ b/HCM2/input/9036_03043900_2022_Student Datasheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/598273eff78d8699/Documents/Irene/DOE SUBMISSIONS HCM2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python\python-projects\HCM2\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="11_2479655579968782E196AE3A21E1ED5DC974BC55" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F40D7031-FD81-4921-9F4F-5F85A3BACAF1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4B4290-A826-419E-B53A-523CB6E40A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2400" yWindow="4215" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,13 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="36" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="97">
   <si>
     <t>Instructions:
 Please fill out the "Student Data" tab for each student included in this system-generated document. For each student, please fill out each column in the template.</t>
@@ -337,9 +337,6 @@
     <t>Main School OPE ID</t>
   </si>
   <si>
-    <t>03043900</t>
-  </si>
-  <si>
     <t>Report Date</t>
   </si>
   <si>
@@ -352,59 +349,41 @@
     <t>2021-2022</t>
   </si>
   <si>
-    <t>KABBANI</t>
-  </si>
-  <si>
-    <t>SUBHI</t>
-  </si>
-  <si>
-    <t>049069401</t>
-  </si>
-  <si>
-    <t>6570 AMBROSIA DR. APT 5102
-MISSION VALLEY, CA 92124</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
-    <t>Rosby</t>
-  </si>
-  <si>
-    <t>Kimaris</t>
-  </si>
-  <si>
-    <t>615866161</t>
-  </si>
-  <si>
-    <t>7555 HIGH STREET APT 24
-LA MESA, CA 91941</t>
-  </si>
-  <si>
-    <t>draper</t>
-  </si>
-  <si>
-    <t>christopher</t>
-  </si>
-  <si>
-    <t>495804833</t>
-  </si>
-  <si>
-    <t>5159 LONGHORN TRL
-FLORISSANT, MO 63033</t>
-  </si>
-  <si>
     <t>Row Labels</t>
   </si>
   <si>
     <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>111111111</t>
+  </si>
+  <si>
+    <t>123 Main st.  Washington, DC 22222</t>
+  </si>
+  <si>
+    <t>111111112</t>
+  </si>
+  <si>
+    <t>124 Main st.  Washington, DC 22222</t>
+  </si>
+  <si>
+    <t>111111113</t>
+  </si>
+  <si>
+    <t>125 Main st.  Washington, DC 22222</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -438,6 +417,17 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -475,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -579,6 +569,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="28"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -914,7 +917,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{90F6BBEE-B2B8-4F78-A2EA-CB174A8EDB08}" name="PivotTable3" cacheId="36" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{90F6BBEE-B2B8-4F78-A2EA-CB174A8EDB08}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="O11:O71" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="29">
     <pivotField axis="axisRow" showAll="0">
@@ -1699,14 +1702,14 @@
   <sheetViews>
     <sheetView zoomScale="80" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58" customWidth="1"/>
     <col min="2" max="2" width="47" customWidth="1"/>
     <col min="3" max="3" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="270.75">
+    <row r="1" spans="1:3" ht="270.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1730,7 +1733,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1740,16 +1743,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="16" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="15" max="15" width="154.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="99.95" customHeight="1">
+    <row r="1" spans="1:29" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1838,7 +1841,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="99.95" customHeight="1">
+    <row r="2" spans="1:29" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1927,7 +1930,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="24.95" customHeight="1">
+    <row r="3" spans="1:29" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -2016,7 +2019,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="50.1" customHeight="1">
+    <row r="4" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -2105,309 +2108,309 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:29">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="O11" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="O12" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="O13" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="O14" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="O15" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="O16" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="15:15">
+    <row r="17" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O17" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="15:15">
+    <row r="18" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O18" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="15:15">
+    <row r="19" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O19" s="13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="15:15">
+    <row r="20" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O20" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="15:15">
+    <row r="21" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O21" s="15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="15:15">
+    <row r="22" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O22" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="15:15">
+    <row r="23" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O23" s="17" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="15:15">
+    <row r="24" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O24" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="15:15">
+    <row r="25" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O25" s="19" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="15:15">
+    <row r="26" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O26" s="20" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="15:15">
+    <row r="27" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O27" s="21" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="15:15">
+    <row r="28" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O28" s="22" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="15:15">
+    <row r="29" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O29" s="23" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="15:15">
+    <row r="30" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O30" s="24" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="15:15">
+    <row r="31" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O31" s="25" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="15:15">
+    <row r="32" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O32" s="26" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="15:15">
+    <row r="33" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O33" s="27" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="15:15">
+    <row r="34" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O34" s="28" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="15:15">
+    <row r="35" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O35" s="29" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="15:15">
+    <row r="36" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O36" s="30" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="15:15">
+    <row r="37" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O37" s="31" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="15:15">
+    <row r="38" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O38" s="32" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="15:15">
+    <row r="39" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O39" s="33" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="15:15">
+    <row r="40" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O40" s="34" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="15:15">
+    <row r="41" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O41" s="35" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="15:15">
+    <row r="42" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O42" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="15:15">
+    <row r="43" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O43" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="15:15">
+    <row r="44" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O44" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="15:15">
+    <row r="45" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O45" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="15:15">
+    <row r="46" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O46" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="15:15">
+    <row r="47" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O47" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="15:15">
+    <row r="48" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O48" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="15:15">
+    <row r="49" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O49" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="15:15">
+    <row r="50" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O50" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="15:15">
+    <row r="51" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O51" s="16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="15:15">
+    <row r="52" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O52" s="17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="15:15">
+    <row r="53" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O53" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="15:15">
+    <row r="54" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O54" s="19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="55" spans="15:15">
+    <row r="55" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O55" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="15:15">
+    <row r="56" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O56" s="21" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="15:15">
+    <row r="57" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O57" s="22" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="15:15">
+    <row r="58" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O58" s="23" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="15:15">
+    <row r="59" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O59" s="24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="15:15">
+    <row r="60" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O60" s="25" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="15:15">
+    <row r="61" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O61" s="26" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="62" spans="15:15">
+    <row r="62" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O62" s="27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="15:15">
+    <row r="63" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O63" s="28" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="15:15">
+    <row r="64" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O64" s="29" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="15:15">
+    <row r="65" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O65" s="30" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="66" spans="15:15">
+    <row r="66" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O66" s="31" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="67" spans="15:15">
+    <row r="67" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O67" s="32" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="68" spans="15:15">
+    <row r="68" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O68" s="33" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="15:15">
+    <row r="69" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O69" s="34" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="15:15">
+    <row r="70" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O70" s="35" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="15:15">
+    <row r="71" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O71" s="7" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2419,14 +2422,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AB10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="16" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="37" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
@@ -2453,7 +2458,7 @@
     <col min="28" max="28" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="25.5">
+    <row r="1" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>80</v>
       </c>
@@ -2461,31 +2466,31 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="5">
+        <v>2222222222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="3" spans="1:28">
-      <c r="A3" s="4" t="s">
-        <v>84</v>
-      </c>
       <c r="B3" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="4" spans="1:28">
-      <c r="A4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28">
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -2495,7 +2500,7 @@
       <c r="C7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="38" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -2571,265 +2576,267 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="38.25">
+    <row r="8" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="B8" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="C8" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="39" t="s">
         <v>91</v>
       </c>
+      <c r="E8" s="40" t="s">
+        <v>92</v>
+      </c>
       <c r="F8" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="R8" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S8" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="T8" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="U8" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="V8" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="W8" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="X8" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Y8" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Z8" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AA8" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AB8" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" ht="25.5">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B9" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="E9" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>96</v>
-      </c>
       <c r="F9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="T9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="U9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="V9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="W9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="X9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Y9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Z9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AA9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AB9" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" ht="25.5">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>100</v>
+      <c r="B10" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="40" t="s">
+        <v>96</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="R10" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S10" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="T10" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="U10" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="V10" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="W10" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="X10" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Y10" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Z10" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AA10" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AB10" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>